<commit_message>
updated the excel file and wait features
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
   <si>
     <t>Adele Rectangular Engineered Wood Coffee Table In Classic Walnut Finish</t>
   </si>
@@ -30,6 +30,114 @@
   </si>
   <si>
     <t>₹14,453</t>
+  </si>
+  <si>
+    <t>Claire Rectangular Solid Wood Coffee Table In Teak Finish</t>
+  </si>
+  <si>
+    <t>₹12,725</t>
+  </si>
+  <si>
+    <t>Tate Square Solid Wood Coffee Table In Teak Finish</t>
+  </si>
+  <si>
+    <t>₹16,554</t>
+  </si>
+  <si>
+    <t>Striado Rectangular Solid Wood Coffee Table In Teak Finish</t>
+  </si>
+  <si>
+    <t>₹10,947</t>
+  </si>
+  <si>
+    <t>Marcel Rectangular Metal Coffee Table In White Gloss Finish</t>
+  </si>
+  <si>
+    <t>₹11,967</t>
+  </si>
+  <si>
+    <t>Renesme Rectangular Solid Wood Coffee Table In Mahogany Finish</t>
+  </si>
+  <si>
+    <t>₹15,317</t>
+  </si>
+  <si>
+    <t>Dyson Abstract Metal Coffee Table In Teak Finish</t>
+  </si>
+  <si>
+    <t>₹7,679</t>
+  </si>
+  <si>
+    <t>Ivara Rectangular Solid Wood Coffee Table In Natural Finish</t>
+  </si>
+  <si>
+    <t>₹16,049</t>
+  </si>
+  <si>
+    <t>Botwin Rectangular Solid Wood Coffee Table In Mahogany Finish</t>
+  </si>
+  <si>
+    <t>₹9,647</t>
+  </si>
+  <si>
+    <t>Zephyr Rectangular Solid Wood Coffee Table In Teak Finish</t>
+  </si>
+  <si>
+    <t>₹14,104</t>
+  </si>
+  <si>
+    <t>Fring Engineered Wood Side Table In Matte Finish</t>
+  </si>
+  <si>
+    <t>₹2,399</t>
+  </si>
+  <si>
+    <t>Claire Rectangular Solid Wood Coffee Table In Mahogany Finish</t>
+  </si>
+  <si>
+    <t>Botwin Rectangular Solid Wood Coffee Table In Teak Finish</t>
+  </si>
+  <si>
+    <t>Epsilon Rectangular Solid Wood Coffee Table In Mahogany Finish</t>
+  </si>
+  <si>
+    <t>₹11,384</t>
+  </si>
+  <si>
+    <t>Dyson Rectangular Metal Coffee Table In Walnut Finish</t>
+  </si>
+  <si>
+    <t>₹10,529</t>
+  </si>
+  <si>
+    <t>Gustowe Rectangular Engineered Wood Coffee Table In Matte Finish</t>
+  </si>
+  <si>
+    <t>₹2,279</t>
+  </si>
+  <si>
+    <t>Striado Rectangular Solid Wood Coffee Table In Mahogany Finish</t>
+  </si>
+  <si>
+    <t>Osiris Rectangular Stone Coffee Table In Finish</t>
+  </si>
+  <si>
+    <t>₹15,677</t>
+  </si>
+  <si>
+    <t>₹8,374</t>
+  </si>
+  <si>
+    <t>Sylvie Rectangular Solid Wood Coffee Table In Natural Finish</t>
+  </si>
+  <si>
+    <t>₹11,839</t>
+  </si>
+  <si>
+    <t>Florence Oval Solid Wood Coffee Table In Teak Finish</t>
+  </si>
+  <si>
+    <t>₹10,223</t>
   </si>
   <si>
     <t/>
@@ -112,215 +220,215 @@
         <v>6</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>6</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>6</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>6</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>6</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>6</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>6</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>6</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>6</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>6</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>6</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>6</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>6</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>6</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>